<commit_message>
[UPDATE] Update full of code for all
</commit_message>
<xml_diff>
--- a/1_CatDog_Project/Compare_CNN/img/validation/PCA/PCA_Validate.xlsx
+++ b/1_CatDog_Project/Compare_CNN/img/validation/PCA/PCA_Validate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\ReviewCV\1_CatDog_Project\Compare_CNN\img\validation\PCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A247000B-6068-4A79-9C58-21207E036753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7560A1-81E0-483B-A996-4725F2BABEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C3EC692A-5CC6-4355-A6E4-DAE0CD00851B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="527" activeTab="1" xr2:uid="{C3EC692A-5CC6-4355-A6E4-DAE0CD00851B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Original</t>
     <phoneticPr fontId="2"/>
@@ -110,6 +110,25 @@
     <t>None</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>Feature dims</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Value difference</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>200 (SIFT + BOVW)</t>
+  </si>
+  <si>
+    <t>200 (SIFT + BOVW)</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
@@ -532,7 +551,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -542,100 +561,115 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -975,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029A3983-9D21-4275-9680-C119F6930BE0}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -987,1309 +1021,1314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="b">
+      <c r="H1" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="25">
         <v>1024</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="10">
         <v>200</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="10">
         <v>800</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="10">
         <v>195</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>30</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="10">
         <v>970</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="10">
         <f t="shared" ref="H2" si="0">SUM(D2,G2)</f>
         <v>1770</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="10">
         <f t="shared" ref="I2" si="1">SUM(D2:G2)</f>
         <v>1995</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="11">
         <f>H2/I2</f>
         <v>0.88721804511278191</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="4">
+      <c r="A3" s="28"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="3">
         <v>300</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>798</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>197</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>26</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>974</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f t="shared" ref="H3:H21" si="2">SUM(D3,G3)</f>
         <v>1772</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <f t="shared" ref="I3:I21" si="3">SUM(D3:G3)</f>
         <v>1995</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <f t="shared" ref="J3:J21" si="4">H3/I3</f>
         <v>0.88822055137844613</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="4">
+      <c r="A4" s="28"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="3">
         <v>400</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>749</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>246</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>30</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>970</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f t="shared" si="2"/>
         <v>1719</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f t="shared" si="4"/>
         <v>0.86165413533834589</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="4">
+      <c r="A5" s="28"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="3">
         <v>500</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>755</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>240</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>28</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>972</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="2"/>
         <v>1727</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <f t="shared" si="4"/>
         <v>0.86566416040100247</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="18">
+      <c r="A6" s="28"/>
+      <c r="B6" s="22">
         <v>4096</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>200</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>779</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>216</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>50</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>950</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f>SUM(D6,G6)</f>
         <v>1729</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f>SUM(D6:G6)</f>
         <v>1995</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <f t="shared" si="4"/>
         <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="4">
+      <c r="A7" s="28"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="3">
         <v>300</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>792</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>203</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>45</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>955</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="2"/>
         <v>1747</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f t="shared" si="4"/>
         <v>0.87568922305764407</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="4">
+      <c r="A8" s="28"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="3">
         <v>400</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>795</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>200</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>34</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>966</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f t="shared" si="2"/>
         <v>1761</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f t="shared" si="4"/>
         <v>0.88270676691729322</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="7">
+      <c r="A9" s="29"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="5">
         <v>500</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>806</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>189</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>32</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>968</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <f t="shared" si="2"/>
         <v>1774</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="6">
         <f t="shared" si="4"/>
         <v>0.88922305764411025</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="25">
         <v>1024</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="10">
         <v>200</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <v>956</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="10">
         <v>39</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="10">
         <v>140</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="10">
         <v>860</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="10">
         <f t="shared" si="2"/>
         <v>1816</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="10">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="11">
         <f t="shared" si="4"/>
         <v>0.91027568922305768</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="4">
+      <c r="A11" s="28"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="3">
         <v>300</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>955</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>40</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>143</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>857</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f t="shared" si="2"/>
         <v>1812</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <f t="shared" si="4"/>
         <v>0.90827067669172934</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="4">
+      <c r="A12" s="28"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="3">
         <v>400</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>954</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>41</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>144</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>856</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f t="shared" si="2"/>
         <v>1810</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <f t="shared" si="4"/>
         <v>0.90726817042606511</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="3"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="4">
+      <c r="A13" s="28"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="3">
         <v>500</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>955</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>40</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>145</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>855</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <f t="shared" si="2"/>
         <v>1810</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <f t="shared" si="4"/>
         <v>0.90726817042606511</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="3"/>
-      <c r="B14" s="18">
+      <c r="A14" s="28"/>
+      <c r="B14" s="22">
         <v>4096</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>200</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>914</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>81</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>175</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>825</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f t="shared" si="2"/>
         <v>1739</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <f t="shared" si="4"/>
         <v>0.8716791979949875</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="4">
+      <c r="A15" s="28"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="3">
         <v>300</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>922</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>73</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>154</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>846</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f t="shared" si="2"/>
         <v>1768</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <f t="shared" si="4"/>
         <v>0.88621553884711779</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="4">
+      <c r="A16" s="28"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="3">
         <v>400</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>925</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>70</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>155</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>845</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f t="shared" si="2"/>
         <v>1770</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="4">
         <f t="shared" si="4"/>
         <v>0.88721804511278191</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A17" s="6"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="7">
+      <c r="A17" s="29"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="5">
         <v>500</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>917</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>78</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <v>157</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="5">
         <v>843</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="5">
         <f t="shared" si="2"/>
         <v>1760</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="5">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="6">
         <f t="shared" si="4"/>
         <v>0.8822055137844611</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="25">
         <v>1024</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="10">
         <v>200</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="10">
         <v>795</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="10">
         <v>200</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <v>39</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="10">
         <v>961</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="10">
         <f t="shared" si="2"/>
         <v>1756</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="10">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="11">
         <f t="shared" si="4"/>
         <v>0.88020050125313287</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="4">
+      <c r="A19" s="28"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="3">
         <v>300</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>787</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>208</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>36</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>964</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <f t="shared" si="2"/>
         <v>1751</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <f t="shared" si="4"/>
         <v>0.87769423558897242</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="4">
+      <c r="A20" s="28"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="3">
         <v>400</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>771</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>224</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>36</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>964</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f t="shared" si="2"/>
         <v>1735</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="4">
         <f t="shared" si="4"/>
         <v>0.86967418546365916</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="4">
+      <c r="A21" s="28"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="3">
         <v>500</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>781</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>214</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>35</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>965</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <f t="shared" si="2"/>
         <v>1746</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <f t="shared" si="3"/>
         <v>1995</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="4">
         <f t="shared" si="4"/>
         <v>0.87518796992481207</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A22" s="3"/>
-      <c r="B22" s="18">
+      <c r="A22" s="28"/>
+      <c r="B22" s="22">
         <v>4096</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>200</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>755</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>240</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>64</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>936</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <f t="shared" ref="H22:H41" si="5">SUM(D22,G22)</f>
         <v>1691</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <f t="shared" ref="I22:I41" si="6">SUM(D22:G22)</f>
         <v>1995</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="4">
         <f t="shared" ref="J22:J41" si="7">H22/I22</f>
         <v>0.84761904761904761</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A23" s="3"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="4">
+      <c r="A23" s="28"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="3">
         <v>300</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>756</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>239</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>53</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>947</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <f t="shared" si="5"/>
         <v>1703</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="4">
         <f t="shared" si="7"/>
         <v>0.85363408521303263</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A24" s="3"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="4">
+      <c r="A24" s="28"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="3">
         <v>400</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>751</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>244</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>45</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>955</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <f t="shared" si="5"/>
         <v>1706</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="4">
         <f t="shared" si="7"/>
         <v>0.85513784461152886</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A25" s="6"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="7">
+      <c r="A25" s="29"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="5">
         <v>500</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>787</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>208</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <v>36</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="5">
         <v>964</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="5">
         <f t="shared" si="5"/>
         <v>1751</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="5">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="6">
         <f t="shared" si="7"/>
         <v>0.87769423558897242</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="25">
         <v>1024</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="10">
         <v>200</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="10">
         <v>1846</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="10">
         <v>140</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="10">
         <v>260</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="10">
         <v>1738</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="10">
         <f t="shared" si="5"/>
         <v>3584</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="10">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="11">
         <f t="shared" si="7"/>
         <v>0.89959839357429716</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A27" s="3"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="4">
+      <c r="A27" s="28"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="3">
         <v>300</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>1853</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>133</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>247</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>1751</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <f t="shared" si="5"/>
         <v>3604</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="3">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="4">
         <f t="shared" si="7"/>
         <v>0.90461847389558236</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A28" s="3"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="4">
+      <c r="A28" s="28"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="3">
         <v>400</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>1836</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>150</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <v>247</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>1751</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <f t="shared" si="5"/>
         <v>3587</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="3">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="4">
         <f t="shared" si="7"/>
         <v>0.90035140562248994</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A29" s="3"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="4">
+      <c r="A29" s="28"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="3">
         <v>500</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>1855</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>131</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="3">
         <v>253</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>1745</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <f t="shared" si="5"/>
         <v>3600</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="3">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="4">
         <f t="shared" si="7"/>
         <v>0.90361445783132532</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A30" s="3"/>
-      <c r="B30" s="18">
+      <c r="A30" s="28"/>
+      <c r="B30" s="22">
         <v>4096</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>200</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>1484</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>502</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>289</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>1709</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <f t="shared" si="5"/>
         <v>3193</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="3">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="4">
         <f t="shared" si="7"/>
         <v>0.80145582329317266</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A31" s="3"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="4">
+      <c r="A31" s="28"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="3">
         <v>300</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>1488</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>498</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <v>278</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>1720</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <f t="shared" si="5"/>
         <v>3208</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="3">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="4">
         <f t="shared" si="7"/>
         <v>0.80522088353413657</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A32" s="3"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="4">
+      <c r="A32" s="28"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="3">
         <v>400</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>1499</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>487</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>264</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>1734</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <f t="shared" si="5"/>
         <v>3233</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="4">
         <f t="shared" si="7"/>
         <v>0.81149598393574296</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A33" s="6"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="7">
+      <c r="A33" s="29"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="5">
         <v>500</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="5">
         <v>1502</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="5">
         <v>484</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="5">
         <v>254</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="5">
         <v>1744</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="5">
         <f t="shared" si="5"/>
         <v>3246</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="5">
         <f t="shared" si="6"/>
         <v>3984</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="6">
         <f t="shared" si="7"/>
         <v>0.81475903614457834</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="25">
         <v>1024</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="10">
         <v>200</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="10">
         <v>921</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="10">
         <v>74</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="10">
         <v>109</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="10">
         <v>891</v>
       </c>
-      <c r="H34" s="13">
+      <c r="H34" s="10">
         <f t="shared" si="5"/>
         <v>1812</v>
       </c>
-      <c r="I34" s="13">
+      <c r="I34" s="10">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J34" s="11">
         <f t="shared" si="7"/>
         <v>0.90827067669172934</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A35" s="3"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="4">
+      <c r="A35" s="28"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="3">
         <v>300</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>914</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>81</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="3">
         <v>110</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>890</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <f t="shared" si="5"/>
         <v>1804</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J35" s="4">
         <f t="shared" si="7"/>
         <v>0.90426065162907265</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A36" s="3"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="4">
+      <c r="A36" s="28"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="3">
         <v>400</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>919</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>76</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <v>114</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>886</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <f t="shared" si="5"/>
         <v>1805</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J36" s="5">
+      <c r="J36" s="4">
         <f t="shared" si="7"/>
         <v>0.90476190476190477</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A37" s="3"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="4">
+      <c r="A37" s="28"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="3">
         <v>500</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>915</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>80</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <v>109</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>891</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f t="shared" si="5"/>
         <v>1806</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J37" s="5">
+      <c r="J37" s="4">
         <f t="shared" si="7"/>
         <v>0.90526315789473688</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A38" s="3"/>
-      <c r="B38" s="18">
+      <c r="A38" s="28"/>
+      <c r="B38" s="22">
         <v>4096</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>200</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <v>829</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>166</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <v>115</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>885</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <f t="shared" si="5"/>
         <v>1714</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J38" s="5">
+      <c r="J38" s="4">
         <f t="shared" si="7"/>
         <v>0.85914786967418544</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A39" s="3"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="4">
+      <c r="A39" s="28"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="3">
         <v>300</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <v>796</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>199</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <v>113</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>887</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <f t="shared" si="5"/>
         <v>1683</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J39" s="4">
         <f t="shared" si="7"/>
         <v>0.84360902255639103</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A40" s="3"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="4">
+      <c r="A40" s="28"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="3">
         <v>400</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>823</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>172</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="3">
         <v>111</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <v>889</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f t="shared" si="5"/>
         <v>1712</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="3">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J40" s="5">
+      <c r="J40" s="4">
         <f t="shared" si="7"/>
         <v>0.85814536340852132</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A41" s="6"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="7">
+      <c r="A41" s="29"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="5">
         <v>500</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="5">
         <v>815</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="5">
         <v>180</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="5">
         <v>111</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="5">
         <v>889</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="5">
         <f t="shared" si="5"/>
         <v>1704</v>
       </c>
-      <c r="I41" s="7">
+      <c r="I41" s="5">
         <f t="shared" si="6"/>
         <v>1995</v>
       </c>
-      <c r="J41" s="8">
+      <c r="J41" s="6">
         <f t="shared" si="7"/>
         <v>0.85413533834586464</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B2:B5"/>
@@ -2300,11 +2339,6 @@
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2316,10 +2350,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D122CD-F01B-4B1F-B903-952B56FC6615}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2329,580 +2363,703 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="29"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="14">
         <v>200</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="14">
         <v>300</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="14">
         <v>400</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="14">
         <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="18">
         <v>1024</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="15">
         <v>0.88721804511278191</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="15">
         <v>0.88822055137844613</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="15">
         <v>0.86165413533834589</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="15">
         <v>0.86566416040100247</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="32"/>
-      <c r="B4" s="28">
+      <c r="A4" s="31"/>
+      <c r="B4" s="19">
         <v>4096</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="16">
         <v>0.8666666666666667</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="16">
         <v>0.87568922305764407</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="16">
         <v>0.88270676691729322</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="16">
         <v>0.88922305764411025</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="18">
         <v>1024</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="15">
         <v>0.91027568922305768</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="15">
         <v>0.90827067669172934</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="15">
         <v>0.90726817042606511</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="15">
         <v>0.90726817042606511</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" s="32"/>
-      <c r="B6" s="28">
+      <c r="A6" s="31"/>
+      <c r="B6" s="19">
         <v>4096</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="16">
         <v>0.8716791979949875</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="16">
         <v>0.88621553884711779</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="16">
         <v>0.88721804511278191</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="16">
         <v>0.8822055137844611</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="18">
         <v>1024</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="15">
         <v>0.88020050125313287</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="15">
         <v>0.87769423558897242</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="15">
         <v>0.86967418546365916</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="15">
         <v>0.87518796992481207</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" s="32"/>
-      <c r="B8" s="28">
+      <c r="A8" s="31"/>
+      <c r="B8" s="19">
         <v>4096</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="16">
         <v>0.84761904761904761</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="16">
         <v>0.85363408521303263</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="16">
         <v>0.85513784461152886</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="16">
         <v>0.87769423558897242</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="18">
         <v>1024</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="15">
         <v>0.89959839357429716</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="15">
         <v>0.90461847389558236</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="15">
         <v>0.90035140562248994</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="15">
         <v>0.90361445783132532</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" s="32"/>
-      <c r="B10" s="28">
+      <c r="A10" s="31"/>
+      <c r="B10" s="19">
         <v>4096</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="16">
         <v>0.80145582329317266</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="16">
         <v>0.80522088353413657</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="16">
         <v>0.81149598393574296</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="16">
         <v>0.81475903614457834</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="18">
         <v>1024</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="15">
         <v>0.90827067669172934</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="15">
         <v>0.90426065162907265</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="15">
         <v>0.90476190476190477</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="15">
         <v>0.90526315789473688</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" s="32"/>
-      <c r="B12" s="28">
+      <c r="A12" s="31"/>
+      <c r="B12" s="19">
         <v>4096</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="16">
         <v>0.85914786967418544</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="16">
         <v>0.84360902255639103</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="16">
         <v>0.85814536340852132</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="16">
         <v>0.85413533834586464</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="29"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="29" t="s">
+      <c r="A17" s="32"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="23"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="14">
         <v>200</v>
       </c>
-      <c r="D18" s="22">
+      <c r="E18" s="14">
         <v>300</v>
       </c>
-      <c r="E18" s="22">
+      <c r="F18" s="14">
         <v>400</v>
       </c>
-      <c r="F18" s="22">
+      <c r="G18" s="14">
         <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="18">
         <v>1024</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="20">
+        <v>0.96089999999999998</v>
+      </c>
+      <c r="D19" s="20">
         <v>0.88721804511278191</v>
       </c>
-      <c r="D19" s="33">
+      <c r="E19" s="20">
         <v>0.88822055137844613</v>
       </c>
-      <c r="E19" s="33">
+      <c r="F19" s="20">
         <v>0.86165413533834589</v>
       </c>
-      <c r="F19" s="33">
+      <c r="G19" s="20">
         <v>0.86566416040100247</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="32"/>
-      <c r="B20" s="28">
+      <c r="A20" s="31"/>
+      <c r="B20" s="19">
         <v>4096</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="21">
+        <v>0.96940000000000004</v>
+      </c>
+      <c r="D20" s="21">
         <v>0.8666666666666667</v>
       </c>
-      <c r="D20" s="34">
+      <c r="E20" s="21">
         <v>0.87568922305764407</v>
       </c>
-      <c r="E20" s="34">
+      <c r="F20" s="21">
         <v>0.88270676691729322</v>
       </c>
-      <c r="F20" s="34">
+      <c r="G20" s="21">
         <v>0.88922305764411025</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="18">
         <v>1024</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="20">
+        <v>0.85660000000000003</v>
+      </c>
+      <c r="D21" s="20">
         <v>0.91027568922305768</v>
       </c>
-      <c r="D21" s="33">
+      <c r="E21" s="20">
         <v>0.90827067669172934</v>
       </c>
-      <c r="E21" s="33">
+      <c r="F21" s="20">
         <v>0.90726817042606511</v>
       </c>
-      <c r="F21" s="33">
+      <c r="G21" s="20">
         <v>0.90726817042606511</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="32"/>
-      <c r="B22" s="28">
+      <c r="A22" s="31"/>
+      <c r="B22" s="19">
         <v>4096</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="21">
+        <v>0.87219999999999998</v>
+      </c>
+      <c r="D22" s="21">
         <v>0.8716791979949875</v>
       </c>
-      <c r="D22" s="34">
+      <c r="E22" s="21">
         <v>0.88621553884711779</v>
       </c>
-      <c r="E22" s="34">
+      <c r="F22" s="21">
         <v>0.88721804511278191</v>
       </c>
-      <c r="F22" s="34">
+      <c r="G22" s="21">
         <v>0.8822055137844611</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="18">
         <v>1024</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="20">
+        <v>0.96140000000000003</v>
+      </c>
+      <c r="D23" s="20">
         <v>0.88020050125313287</v>
       </c>
-      <c r="D23" s="33">
+      <c r="E23" s="20">
         <v>0.87769423558897242</v>
       </c>
-      <c r="E23" s="33">
+      <c r="F23" s="20">
         <v>0.86967418546365916</v>
       </c>
-      <c r="F23" s="33">
+      <c r="G23" s="20">
         <v>0.87518796992481207</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="32"/>
-      <c r="B24" s="28">
+      <c r="A24" s="31"/>
+      <c r="B24" s="19">
         <v>4096</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="21">
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="D24" s="21">
         <v>0.84761904761904761</v>
       </c>
-      <c r="D24" s="34">
+      <c r="E24" s="21">
         <v>0.85363408521303263</v>
       </c>
-      <c r="E24" s="34">
+      <c r="F24" s="21">
         <v>0.85513784461152886</v>
       </c>
-      <c r="F24" s="34">
+      <c r="G24" s="21">
         <v>0.87769423558897242</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="18">
         <v>1024</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="20">
+        <v>0.86839999999999995</v>
+      </c>
+      <c r="D25" s="20">
         <v>0.89959839357429716</v>
       </c>
-      <c r="D25" s="33">
+      <c r="E25" s="20">
         <v>0.90461847389558236</v>
       </c>
-      <c r="E25" s="33">
+      <c r="F25" s="20">
         <v>0.90035140562248994</v>
       </c>
-      <c r="F25" s="33">
+      <c r="G25" s="20">
         <v>0.90361445783132532</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="32"/>
-      <c r="B26" s="28">
+      <c r="A26" s="31"/>
+      <c r="B26" s="19">
         <v>4096</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="21">
+        <v>0.86040000000000005</v>
+      </c>
+      <c r="D26" s="21">
         <v>0.80145582329317266</v>
       </c>
-      <c r="D26" s="34">
+      <c r="E26" s="21">
         <v>0.80522088353413657</v>
       </c>
-      <c r="E26" s="34">
+      <c r="F26" s="21">
         <v>0.81149598393574296</v>
       </c>
-      <c r="F26" s="34">
+      <c r="G26" s="21">
         <v>0.81475903614457834</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="18">
         <v>1024</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="20">
+        <v>0.89370000000000005</v>
+      </c>
+      <c r="D27" s="20">
         <v>0.90827067669172934</v>
       </c>
-      <c r="D27" s="33">
+      <c r="E27" s="20">
         <v>0.90426065162907265</v>
       </c>
-      <c r="E27" s="33">
+      <c r="F27" s="20">
         <v>0.90476190476190477</v>
       </c>
-      <c r="F27" s="33">
+      <c r="G27" s="20">
         <v>0.90526315789473688</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="32"/>
-      <c r="B28" s="28">
+      <c r="A28" s="31"/>
+      <c r="B28" s="19">
         <v>4096</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="21">
+        <v>0.9042</v>
+      </c>
+      <c r="D28" s="21">
         <v>0.85914786967418544</v>
       </c>
-      <c r="D28" s="34">
+      <c r="E28" s="21">
         <v>0.84360902255639103</v>
       </c>
-      <c r="E28" s="34">
+      <c r="F28" s="21">
         <v>0.85814536340852132</v>
       </c>
-      <c r="F28" s="34">
+      <c r="G28" s="21">
         <v>0.85413533834586464</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="29"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="29" t="s">
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="23"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A33" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="22" t="s">
+      <c r="A33" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="12">
         <v>200</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="12">
         <v>300</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="12">
         <v>400</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="12">
         <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="12">
         <v>1024</v>
       </c>
-      <c r="C34" s="33">
+      <c r="C34" s="36">
         <v>0.70306405999999999</v>
       </c>
-      <c r="D34" s="33">
+      <c r="D34" s="36">
         <v>0.70055710000000004</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="36">
         <v>0.70445681999999998</v>
       </c>
-      <c r="F34" s="33">
+      <c r="F34" s="36">
         <v>0.69860723999999996</v>
       </c>
-      <c r="G34" s="33">
+      <c r="G34" s="36">
         <v>0.69972144000000003</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A35" s="32"/>
-      <c r="B35" s="28">
+      <c r="A35" s="35"/>
+      <c r="B35" s="12">
         <v>4096</v>
       </c>
-      <c r="C35" s="34">
+      <c r="C35" s="36">
         <v>0.71949799999999997</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35" s="36">
         <v>0.68077989999999999</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>0.68662951999999999</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="36">
         <v>0.68412256000000005</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="36">
         <v>0.68746518000000001</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="35"/>
+      <c r="B36" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="37">
+        <v>0.70724229999999999</v>
+      </c>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A37" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B37" s="12">
         <v>1024</v>
       </c>
-      <c r="C36" s="33">
+      <c r="C37" s="36">
         <v>0.90170511529999997</v>
       </c>
-      <c r="D36" s="33">
+      <c r="D37" s="36">
         <v>0.89593781299999997</v>
       </c>
-      <c r="E36" s="33">
+      <c r="E37" s="36">
         <v>0.89827816000000005</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F37" s="36">
         <v>0.89894684000000002</v>
       </c>
-      <c r="G36" s="33">
+      <c r="G37" s="36">
         <v>0.90003343000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A37" s="32"/>
-      <c r="B37" s="28">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A38" s="35"/>
+      <c r="B38" s="12">
         <v>4096</v>
       </c>
-      <c r="C37" s="34">
+      <c r="C38" s="36">
         <v>0.91014710789999997</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D38" s="36">
         <v>0.87771648000000002</v>
       </c>
-      <c r="E37" s="34">
+      <c r="E38" s="36">
         <v>0.88749582000000005</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F38" s="36">
         <v>0.89175859999999996</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G38" s="36">
         <v>0.89660647999999998</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A39" s="35"/>
+      <c r="B39" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="37">
+        <v>0.72116340000000001</v>
+      </c>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A40" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="12">
+        <v>1024</v>
+      </c>
+      <c r="C40" s="38">
+        <f>C37-C34</f>
+        <v>0.19864105529999998</v>
+      </c>
+      <c r="D40" s="38">
+        <f t="shared" ref="D40:G41" si="0">D37-D34</f>
+        <v>0.19538071299999993</v>
+      </c>
+      <c r="E40" s="38">
+        <f t="shared" si="0"/>
+        <v>0.19382134000000006</v>
+      </c>
+      <c r="F40" s="38">
+        <f t="shared" si="0"/>
+        <v>0.20033960000000006</v>
+      </c>
+      <c r="G40" s="38">
+        <f t="shared" si="0"/>
+        <v>0.20031199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A41" s="35"/>
+      <c r="B41" s="12">
+        <v>4096</v>
+      </c>
+      <c r="C41" s="38">
+        <f>C38-C35</f>
+        <v>0.1906491079</v>
+      </c>
+      <c r="D41" s="38">
+        <f>D38-D35</f>
+        <v>0.19693658000000003</v>
+      </c>
+      <c r="E41" s="38">
+        <f>E38-E35</f>
+        <v>0.20086630000000005</v>
+      </c>
+      <c r="F41" s="38">
+        <f>F38-F35</f>
+        <v>0.20763603999999991</v>
+      </c>
+      <c r="G41" s="38">
+        <f>G38-G35</f>
+        <v>0.20914129999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A42" s="35"/>
+      <c r="B42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="39">
+        <f>C39-C36</f>
+        <v>1.392110000000002E-2</v>
+      </c>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A32:B32"/>
+  <mergeCells count="22">
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C42:G42"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
@@ -2910,6 +3067,15 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>